<commit_message>
more fixes and tests for frequency dependent s-parameter models
</commit_message>
<xml_diff>
--- a/TestSignalIntegrity/FourPortTline.xlsx
+++ b/TestSignalIntegrity/FourPortTline.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="33">
   <si>
     <t>mA</t>
   </si>
@@ -68,12 +68,63 @@
   <si>
     <t>V R4</t>
   </si>
+  <si>
+    <t>A L1</t>
+  </si>
+  <si>
+    <t>B L1</t>
+  </si>
+  <si>
+    <t>A L3</t>
+  </si>
+  <si>
+    <t>B L3</t>
+  </si>
+  <si>
+    <t>A L2</t>
+  </si>
+  <si>
+    <t>B L2</t>
+  </si>
+  <si>
+    <t>A L4</t>
+  </si>
+  <si>
+    <t>B L4</t>
+  </si>
+  <si>
+    <t>A R1</t>
+  </si>
+  <si>
+    <t>B R1</t>
+  </si>
+  <si>
+    <t>A R3</t>
+  </si>
+  <si>
+    <t>B R3</t>
+  </si>
+  <si>
+    <t>A R2</t>
+  </si>
+  <si>
+    <t>B R2</t>
+  </si>
+  <si>
+    <t>A R4</t>
+  </si>
+  <si>
+    <t>B R4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +140,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,17 +170,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AF21"/>
+  <dimension ref="B1:AW21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AL24" sqref="AL24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,7 +509,12 @@
     <col min="32" max="32" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="AH1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:49" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
@@ -488,8 +560,56 @@
       <c r="AE3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="AH3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AT3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2.5000000000000002E-10</v>
       </c>
@@ -583,8 +703,72 @@
       <c r="AF4" t="s">
         <v>1</v>
       </c>
+      <c r="AH4" s="4">
+        <f>U4+$AH$1*E4/1000</f>
+        <v>0.99999965000000002</v>
+      </c>
+      <c r="AI4" s="4">
+        <f>U4-$AH$1*E4/1000</f>
+        <v>0.33335835000000003</v>
+      </c>
+      <c r="AJ4" s="4">
+        <f>W4+$AH$1*G4/1000</f>
+        <v>3.4999999998230891E-7</v>
+      </c>
+      <c r="AK4" s="4">
+        <f>W4-$AH$1*G4/1000</f>
+        <v>0.66664164999999997</v>
+      </c>
+      <c r="AL4" s="3">
+        <f>Y4+$AH$1*I4/1000</f>
+        <v>3.7499999999999997E-6</v>
+      </c>
+      <c r="AM4" s="3">
+        <f>Y4-$AH$1*I4/1000</f>
+        <v>1.225E-5</v>
+      </c>
+      <c r="AN4" s="3">
+        <f>AA4+$AH$1*K4/1000</f>
+        <v>4.25E-6</v>
+      </c>
+      <c r="AO4" s="3">
+        <f>AA4-$AH$1*K4/1000</f>
+        <v>-4.25E-6</v>
+      </c>
+      <c r="AP4" s="3">
+        <f>Y4+$AH$1*M4/1000</f>
+        <v>1.225E-5</v>
+      </c>
+      <c r="AQ4" s="3">
+        <f>Y4-$AH$1*M4/1000</f>
+        <v>3.7499999999999997E-6</v>
+      </c>
+      <c r="AR4" s="3">
+        <f>AA4+$AH$1*O4/1000</f>
+        <v>-4.25E-6</v>
+      </c>
+      <c r="AS4" s="3">
+        <f>AA4-$AH$1*O4/1000</f>
+        <v>4.25E-6</v>
+      </c>
+      <c r="AT4" s="3">
+        <f>AC4+$AH$1*Q4/1000</f>
+        <v>-2.5000000000000015E-7</v>
+      </c>
+      <c r="AU4" s="3">
+        <f>AC4-$AH$1*Q4/1000</f>
+        <v>8.2500000000000006E-6</v>
+      </c>
+      <c r="AV4" s="3">
+        <f>AE4+$AH$1*S4/1000</f>
+        <v>2.5000000000000015E-7</v>
+      </c>
+      <c r="AW4" s="3">
+        <f>AE4-$AH$1*S4/1000</f>
+        <v>-8.2500000000000006E-6</v>
+      </c>
     </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>7.5E-10</v>
       </c>
@@ -678,8 +862,72 @@
       <c r="AF5" t="s">
         <v>1</v>
       </c>
+      <c r="AH5" s="3">
+        <f t="shared" ref="AH5:AH21" si="0">U5+$AH$1*E5/1000</f>
+        <v>0.99999965000000002</v>
+      </c>
+      <c r="AI5" s="3">
+        <f t="shared" ref="AI5:AI21" si="1">U5-$AH$1*E5/1000</f>
+        <v>0.33335835000000003</v>
+      </c>
+      <c r="AJ5" s="3">
+        <f t="shared" ref="AJ5:AJ21" si="2">W5+$AH$1*G5/1000</f>
+        <v>3.4999999998230891E-7</v>
+      </c>
+      <c r="AK5" s="3">
+        <f t="shared" ref="AK5:AK21" si="3">W5-$AH$1*G5/1000</f>
+        <v>0.66664164999999997</v>
+      </c>
+      <c r="AL5" s="4">
+        <f t="shared" ref="AL5:AL21" si="4">Y5+$AH$1*I5/1000</f>
+        <v>4.450000000044696E-6</v>
+      </c>
+      <c r="AM5" s="4">
+        <f t="shared" ref="AM5:AM21" si="5">Y5-$AH$1*I5/1000</f>
+        <v>0.66667955000000001</v>
+      </c>
+      <c r="AN5" s="4">
+        <f t="shared" ref="AN5:AN21" si="6">AA5+$AH$1*K5/1000</f>
+        <v>0.33333754999999998</v>
+      </c>
+      <c r="AO5" s="4">
+        <f t="shared" ref="AO5:AO21" si="7">AA5-$AH$1*K5/1000</f>
+        <v>-0.33333754999999998</v>
+      </c>
+      <c r="AP5" s="4">
+        <f t="shared" ref="AP5:AP21" si="8">Y5+$AH$1*M5/1000</f>
+        <v>0.66667955000000001</v>
+      </c>
+      <c r="AQ5" s="4">
+        <f t="shared" ref="AQ5:AQ21" si="9">Y5-$AH$1*M5/1000</f>
+        <v>4.450000000044696E-6</v>
+      </c>
+      <c r="AR5" s="4">
+        <f t="shared" ref="AR5:AR21" si="10">AA5+$AH$1*O5/1000</f>
+        <v>-0.33333754999999998</v>
+      </c>
+      <c r="AS5" s="4">
+        <f t="shared" ref="AS5:AS21" si="11">AA5-$AH$1*O5/1000</f>
+        <v>0.33333754999999998</v>
+      </c>
+      <c r="AT5" s="3">
+        <f t="shared" ref="AT5:AT21" si="12">AC5+$AH$1*Q5/1000</f>
+        <v>-2.5000000000000015E-7</v>
+      </c>
+      <c r="AU5" s="3">
+        <f t="shared" ref="AU5:AU21" si="13">AC5-$AH$1*Q5/1000</f>
+        <v>8.2500000000000006E-6</v>
+      </c>
+      <c r="AV5" s="3">
+        <f t="shared" ref="AV5:AV21" si="14">AE5+$AH$1*S5/1000</f>
+        <v>2.5000000000000015E-7</v>
+      </c>
+      <c r="AW5" s="3">
+        <f t="shared" ref="AW5:AW21" si="15">AE5-$AH$1*S5/1000</f>
+        <v>-8.2500000000000006E-6</v>
+      </c>
     </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1.25E-9</v>
       </c>
@@ -773,8 +1021,72 @@
       <c r="AF6" t="s">
         <v>1</v>
       </c>
+      <c r="AH6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999965000000002</v>
+      </c>
+      <c r="AI6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33335835000000003</v>
+      </c>
+      <c r="AJ6" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4999999998230891E-7</v>
+      </c>
+      <c r="AK6" s="3">
+        <f t="shared" si="3"/>
+        <v>0.66664164999999997</v>
+      </c>
+      <c r="AL6" s="3">
+        <f t="shared" si="4"/>
+        <v>4.450000000044696E-6</v>
+      </c>
+      <c r="AM6" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66667955000000001</v>
+      </c>
+      <c r="AN6" s="3">
+        <f t="shared" si="6"/>
+        <v>0.33333754999999998</v>
+      </c>
+      <c r="AO6" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.33333754999999998</v>
+      </c>
+      <c r="AP6" s="3">
+        <f t="shared" si="8"/>
+        <v>0.66667955000000001</v>
+      </c>
+      <c r="AQ6" s="3">
+        <f t="shared" si="9"/>
+        <v>4.450000000044696E-6</v>
+      </c>
+      <c r="AR6" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.33333754999999998</v>
+      </c>
+      <c r="AS6" s="3">
+        <f t="shared" si="11"/>
+        <v>0.33333754999999998</v>
+      </c>
+      <c r="AT6" s="4">
+        <f t="shared" si="12"/>
+        <v>-4.4999999998518447E-7</v>
+      </c>
+      <c r="AU6" s="4">
+        <f t="shared" si="13"/>
+        <v>0.44445245</v>
+      </c>
+      <c r="AV6" s="4">
+        <f t="shared" si="14"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AW6" s="4">
+        <f t="shared" si="15"/>
+        <v>-0.44445245</v>
+      </c>
     </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>1.75E-9</v>
       </c>
@@ -868,8 +1180,72 @@
       <c r="AF7" t="s">
         <v>1</v>
       </c>
+      <c r="AH7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999965000000002</v>
+      </c>
+      <c r="AI7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.33335835000000003</v>
+      </c>
+      <c r="AJ7" s="3">
+        <f t="shared" si="2"/>
+        <v>3.4999999998230891E-7</v>
+      </c>
+      <c r="AK7" s="3">
+        <f t="shared" si="3"/>
+        <v>0.66664164999999997</v>
+      </c>
+      <c r="AL7" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22222654999999999</v>
+      </c>
+      <c r="AM7" s="4">
+        <f t="shared" si="5"/>
+        <v>0.66667944999999995</v>
+      </c>
+      <c r="AN7" s="4">
+        <f t="shared" si="6"/>
+        <v>0.22222644999999999</v>
+      </c>
+      <c r="AO7" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.22222644999999999</v>
+      </c>
+      <c r="AP7" s="4">
+        <f t="shared" si="8"/>
+        <v>0.66667944999999995</v>
+      </c>
+      <c r="AQ7" s="4">
+        <f t="shared" si="9"/>
+        <v>0.22222654999999999</v>
+      </c>
+      <c r="AR7" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.22222644999999999</v>
+      </c>
+      <c r="AS7" s="4">
+        <f t="shared" si="11"/>
+        <v>0.22222644999999999</v>
+      </c>
+      <c r="AT7" s="3">
+        <f t="shared" si="12"/>
+        <v>-4.4999999998518447E-7</v>
+      </c>
+      <c r="AU7" s="3">
+        <f t="shared" si="13"/>
+        <v>0.44445245</v>
+      </c>
+      <c r="AV7" s="3">
+        <f t="shared" si="14"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AW7" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.44445245</v>
+      </c>
     </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>2.2499999999999999E-9</v>
       </c>
@@ -963,8 +1339,72 @@
       <c r="AF8" t="s">
         <v>1</v>
       </c>
+      <c r="AH8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99999955000000007</v>
+      </c>
+      <c r="AI8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48150644999999997</v>
+      </c>
+      <c r="AJ8" s="4">
+        <f t="shared" si="2"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AK8" s="4">
+        <f t="shared" si="3"/>
+        <v>0.51849355000000008</v>
+      </c>
+      <c r="AL8" s="3">
+        <f t="shared" si="4"/>
+        <v>0.22222654999999999</v>
+      </c>
+      <c r="AM8" s="3">
+        <f t="shared" si="5"/>
+        <v>0.66667944999999995</v>
+      </c>
+      <c r="AN8" s="3">
+        <f t="shared" si="6"/>
+        <v>0.22222644999999999</v>
+      </c>
+      <c r="AO8" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.22222644999999999</v>
+      </c>
+      <c r="AP8" s="3">
+        <f t="shared" si="8"/>
+        <v>0.66667944999999995</v>
+      </c>
+      <c r="AQ8" s="3">
+        <f t="shared" si="9"/>
+        <v>0.22222654999999999</v>
+      </c>
+      <c r="AR8" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.22222644999999999</v>
+      </c>
+      <c r="AS8" s="3">
+        <f t="shared" si="11"/>
+        <v>0.22222644999999999</v>
+      </c>
+      <c r="AT8" s="3">
+        <f t="shared" si="12"/>
+        <v>-4.4999999998518447E-7</v>
+      </c>
+      <c r="AU8" s="3">
+        <f t="shared" si="13"/>
+        <v>0.44445245</v>
+      </c>
+      <c r="AV8" s="3">
+        <f t="shared" si="14"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AW8" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.44445245</v>
+      </c>
     </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>2.7499999999999998E-9</v>
       </c>
@@ -1058,8 +1498,72 @@
       <c r="AF9" t="s">
         <v>1</v>
       </c>
+      <c r="AH9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999955000000007</v>
+      </c>
+      <c r="AI9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.48150644999999997</v>
+      </c>
+      <c r="AJ9" s="3">
+        <f t="shared" si="2"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AK9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.51849355000000008</v>
+      </c>
+      <c r="AL9" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22222649999999994</v>
+      </c>
+      <c r="AM9" s="4">
+        <f t="shared" si="5"/>
+        <v>0.74075350000000006</v>
+      </c>
+      <c r="AN9" s="4">
+        <f t="shared" si="6"/>
+        <v>0.25926350000000004</v>
+      </c>
+      <c r="AO9" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.25926350000000004</v>
+      </c>
+      <c r="AP9" s="4">
+        <f t="shared" si="8"/>
+        <v>0.74075350000000006</v>
+      </c>
+      <c r="AQ9" s="4">
+        <f t="shared" si="9"/>
+        <v>0.22222649999999994</v>
+      </c>
+      <c r="AR9" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.25926350000000004</v>
+      </c>
+      <c r="AS9" s="4">
+        <f t="shared" si="11"/>
+        <v>0.25926350000000004</v>
+      </c>
+      <c r="AT9" s="3">
+        <f t="shared" si="12"/>
+        <v>-4.4999999998518447E-7</v>
+      </c>
+      <c r="AU9" s="3">
+        <f t="shared" si="13"/>
+        <v>0.44445245</v>
+      </c>
+      <c r="AV9" s="3">
+        <f t="shared" si="14"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AW9" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.44445245</v>
+      </c>
     </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>3.2500000000000002E-9</v>
       </c>
@@ -1153,8 +1657,72 @@
       <c r="AF10" t="s">
         <v>1</v>
       </c>
+      <c r="AH10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999955000000007</v>
+      </c>
+      <c r="AI10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.48150644999999997</v>
+      </c>
+      <c r="AJ10" s="3">
+        <f t="shared" si="2"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AK10" s="3">
+        <f t="shared" si="3"/>
+        <v>0.51849355000000008</v>
+      </c>
+      <c r="AL10" s="3">
+        <f t="shared" si="4"/>
+        <v>0.22222649999999994</v>
+      </c>
+      <c r="AM10" s="3">
+        <f t="shared" si="5"/>
+        <v>0.74075350000000006</v>
+      </c>
+      <c r="AN10" s="3">
+        <f t="shared" si="6"/>
+        <v>0.25926350000000004</v>
+      </c>
+      <c r="AO10" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.25926350000000004</v>
+      </c>
+      <c r="AP10" s="3">
+        <f t="shared" si="8"/>
+        <v>0.74075350000000006</v>
+      </c>
+      <c r="AQ10" s="3">
+        <f t="shared" si="9"/>
+        <v>0.22222649999999994</v>
+      </c>
+      <c r="AR10" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.25926350000000004</v>
+      </c>
+      <c r="AS10" s="3">
+        <f t="shared" si="11"/>
+        <v>0.25926350000000004</v>
+      </c>
+      <c r="AT10" s="4">
+        <f t="shared" si="12"/>
+        <v>2.0000000000575113E-7</v>
+      </c>
+      <c r="AU10" s="4">
+        <f t="shared" si="13"/>
+        <v>0.49383579999999999</v>
+      </c>
+      <c r="AV10" s="4">
+        <f t="shared" si="14"/>
+        <v>-2.0000000000575113E-7</v>
+      </c>
+      <c r="AW10" s="4">
+        <f t="shared" si="15"/>
+        <v>-0.49383579999999999</v>
+      </c>
     </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>3.7499999999999997E-9</v>
       </c>
@@ -1248,8 +1816,72 @@
       <c r="AF11" t="s">
         <v>1</v>
       </c>
+      <c r="AH11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999955000000007</v>
+      </c>
+      <c r="AI11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.48150644999999997</v>
+      </c>
+      <c r="AJ11" s="3">
+        <f t="shared" si="2"/>
+        <v>4.4999999998518447E-7</v>
+      </c>
+      <c r="AK11" s="3">
+        <f t="shared" si="3"/>
+        <v>0.51849355000000008</v>
+      </c>
+      <c r="AL11" s="4">
+        <f t="shared" si="4"/>
+        <v>0.2469182</v>
+      </c>
+      <c r="AM11" s="4">
+        <f t="shared" si="5"/>
+        <v>0.74075380000000002</v>
+      </c>
+      <c r="AN11" s="4">
+        <f t="shared" si="6"/>
+        <v>0.24691779999999999</v>
+      </c>
+      <c r="AO11" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.24691779999999999</v>
+      </c>
+      <c r="AP11" s="4">
+        <f t="shared" si="8"/>
+        <v>0.74075380000000002</v>
+      </c>
+      <c r="AQ11" s="4">
+        <f t="shared" si="9"/>
+        <v>0.2469182</v>
+      </c>
+      <c r="AR11" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.24691779999999999</v>
+      </c>
+      <c r="AS11" s="4">
+        <f t="shared" si="11"/>
+        <v>0.24691779999999999</v>
+      </c>
+      <c r="AT11" s="3">
+        <f t="shared" si="12"/>
+        <v>2.0000000000575113E-7</v>
+      </c>
+      <c r="AU11" s="3">
+        <f t="shared" si="13"/>
+        <v>0.49383579999999999</v>
+      </c>
+      <c r="AV11" s="3">
+        <f t="shared" si="14"/>
+        <v>-2.0000000000575113E-7</v>
+      </c>
+      <c r="AW11" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.49383579999999999</v>
+      </c>
     </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>4.25E-9</v>
       </c>
@@ -1343,8 +1975,72 @@
       <c r="AF12" t="s">
         <v>1</v>
       </c>
+      <c r="AH12" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0000001000000001</v>
+      </c>
+      <c r="AI12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.49796789999999996</v>
+      </c>
+      <c r="AJ12" s="4">
+        <f t="shared" si="2"/>
+        <v>-1.0000000000287557E-7</v>
+      </c>
+      <c r="AK12" s="4">
+        <f t="shared" si="3"/>
+        <v>0.50203210000000009</v>
+      </c>
+      <c r="AL12" s="3">
+        <f t="shared" si="4"/>
+        <v>0.2469182</v>
+      </c>
+      <c r="AM12" s="3">
+        <f t="shared" si="5"/>
+        <v>0.74075380000000002</v>
+      </c>
+      <c r="AN12" s="3">
+        <f t="shared" si="6"/>
+        <v>0.24691779999999999</v>
+      </c>
+      <c r="AO12" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.24691779999999999</v>
+      </c>
+      <c r="AP12" s="3">
+        <f t="shared" si="8"/>
+        <v>0.74075380000000002</v>
+      </c>
+      <c r="AQ12" s="3">
+        <f t="shared" si="9"/>
+        <v>0.2469182</v>
+      </c>
+      <c r="AR12" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.24691779999999999</v>
+      </c>
+      <c r="AS12" s="3">
+        <f t="shared" si="11"/>
+        <v>0.24691779999999999</v>
+      </c>
+      <c r="AT12" s="3">
+        <f t="shared" si="12"/>
+        <v>2.0000000000575113E-7</v>
+      </c>
+      <c r="AU12" s="3">
+        <f t="shared" si="13"/>
+        <v>0.49383579999999999</v>
+      </c>
+      <c r="AV12" s="3">
+        <f t="shared" si="14"/>
+        <v>-2.0000000000575113E-7</v>
+      </c>
+      <c r="AW12" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.49383579999999999</v>
+      </c>
     </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>4.7500000000000003E-9</v>
       </c>
@@ -1438,8 +2134,72 @@
       <c r="AF13" t="s">
         <v>1</v>
       </c>
+      <c r="AH13" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0000001000000001</v>
+      </c>
+      <c r="AI13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49796789999999996</v>
+      </c>
+      <c r="AJ13" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.0000000000287557E-7</v>
+      </c>
+      <c r="AK13" s="3">
+        <f t="shared" si="3"/>
+        <v>0.50203210000000009</v>
+      </c>
+      <c r="AL13" s="4">
+        <f t="shared" si="4"/>
+        <v>0.24691795</v>
+      </c>
+      <c r="AM13" s="4">
+        <f t="shared" si="5"/>
+        <v>0.74898405000000001</v>
+      </c>
+      <c r="AN13" s="4">
+        <f t="shared" si="6"/>
+        <v>0.25103304999999998</v>
+      </c>
+      <c r="AO13" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.25103304999999998</v>
+      </c>
+      <c r="AP13" s="4">
+        <f t="shared" si="8"/>
+        <v>0.74898405000000001</v>
+      </c>
+      <c r="AQ13" s="4">
+        <f t="shared" si="9"/>
+        <v>0.24691795</v>
+      </c>
+      <c r="AR13" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.25103304999999998</v>
+      </c>
+      <c r="AS13" s="4">
+        <f t="shared" si="11"/>
+        <v>0.25103304999999998</v>
+      </c>
+      <c r="AT13" s="3">
+        <f t="shared" si="12"/>
+        <v>2.0000000000575113E-7</v>
+      </c>
+      <c r="AU13" s="3">
+        <f t="shared" si="13"/>
+        <v>0.49383579999999999</v>
+      </c>
+      <c r="AV13" s="3">
+        <f t="shared" si="14"/>
+        <v>-2.0000000000575113E-7</v>
+      </c>
+      <c r="AW13" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.49383579999999999</v>
+      </c>
     </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>5.2499999999999999E-9</v>
       </c>
@@ -1533,8 +2293,72 @@
       <c r="AF14" t="s">
         <v>1</v>
       </c>
+      <c r="AH14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0000001000000001</v>
+      </c>
+      <c r="AI14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49796789999999996</v>
+      </c>
+      <c r="AJ14" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.0000000000287557E-7</v>
+      </c>
+      <c r="AK14" s="3">
+        <f t="shared" si="3"/>
+        <v>0.50203210000000009</v>
+      </c>
+      <c r="AL14" s="3">
+        <f t="shared" si="4"/>
+        <v>0.24691795</v>
+      </c>
+      <c r="AM14" s="3">
+        <f t="shared" si="5"/>
+        <v>0.74898405000000001</v>
+      </c>
+      <c r="AN14" s="3">
+        <f t="shared" si="6"/>
+        <v>0.25103304999999998</v>
+      </c>
+      <c r="AO14" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.25103304999999998</v>
+      </c>
+      <c r="AP14" s="3">
+        <f t="shared" si="8"/>
+        <v>0.74898405000000001</v>
+      </c>
+      <c r="AQ14" s="3">
+        <f t="shared" si="9"/>
+        <v>0.24691795</v>
+      </c>
+      <c r="AR14" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.25103304999999998</v>
+      </c>
+      <c r="AS14" s="3">
+        <f t="shared" si="11"/>
+        <v>0.25103304999999998</v>
+      </c>
+      <c r="AT14" s="4">
+        <f t="shared" si="12"/>
+        <v>-2.9999999998087112E-7</v>
+      </c>
+      <c r="AU14" s="4">
+        <f t="shared" si="13"/>
+        <v>0.4993223</v>
+      </c>
+      <c r="AV14" s="4">
+        <f t="shared" si="14"/>
+        <v>2.9999999998087112E-7</v>
+      </c>
+      <c r="AW14" s="4">
+        <f t="shared" si="15"/>
+        <v>-0.4993223</v>
+      </c>
     </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>5.7500000000000002E-9</v>
       </c>
@@ -1628,8 +2452,72 @@
       <c r="AF15" t="s">
         <v>1</v>
       </c>
+      <c r="AH15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0000001000000001</v>
+      </c>
+      <c r="AI15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49796789999999996</v>
+      </c>
+      <c r="AJ15" s="3">
+        <f t="shared" si="2"/>
+        <v>-1.0000000000287557E-7</v>
+      </c>
+      <c r="AK15" s="3">
+        <f t="shared" si="3"/>
+        <v>0.50203210000000009</v>
+      </c>
+      <c r="AL15" s="4">
+        <f t="shared" si="4"/>
+        <v>0.24966170000000004</v>
+      </c>
+      <c r="AM15" s="4">
+        <f t="shared" si="5"/>
+        <v>0.74898430000000005</v>
+      </c>
+      <c r="AN15" s="4">
+        <f t="shared" si="6"/>
+        <v>0.24966129999999997</v>
+      </c>
+      <c r="AO15" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.24966129999999997</v>
+      </c>
+      <c r="AP15" s="4">
+        <f t="shared" si="8"/>
+        <v>0.74898430000000005</v>
+      </c>
+      <c r="AQ15" s="4">
+        <f t="shared" si="9"/>
+        <v>0.24966170000000004</v>
+      </c>
+      <c r="AR15" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.24966129999999997</v>
+      </c>
+      <c r="AS15" s="4">
+        <f t="shared" si="11"/>
+        <v>0.24966129999999997</v>
+      </c>
+      <c r="AT15" s="3">
+        <f t="shared" si="12"/>
+        <v>-2.9999999998087112E-7</v>
+      </c>
+      <c r="AU15" s="3">
+        <f t="shared" si="13"/>
+        <v>0.4993223</v>
+      </c>
+      <c r="AV15" s="3">
+        <f t="shared" si="14"/>
+        <v>2.9999999998087112E-7</v>
+      </c>
+      <c r="AW15" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.4993223</v>
+      </c>
     </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>6.2499999999999997E-9</v>
       </c>
@@ -1723,8 +2611,72 @@
       <c r="AF16" t="s">
         <v>1</v>
       </c>
+      <c r="AH16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99999959999999999</v>
+      </c>
+      <c r="AI16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.49979639999999997</v>
+      </c>
+      <c r="AJ16" s="4">
+        <f t="shared" si="2"/>
+        <v>4.0000000001150227E-7</v>
+      </c>
+      <c r="AK16" s="4">
+        <f t="shared" si="3"/>
+        <v>0.50020359999999997</v>
+      </c>
+      <c r="AL16" s="3">
+        <f t="shared" si="4"/>
+        <v>0.24966170000000004</v>
+      </c>
+      <c r="AM16" s="3">
+        <f t="shared" si="5"/>
+        <v>0.74898430000000005</v>
+      </c>
+      <c r="AN16" s="3">
+        <f t="shared" si="6"/>
+        <v>0.24966129999999997</v>
+      </c>
+      <c r="AO16" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.24966129999999997</v>
+      </c>
+      <c r="AP16" s="3">
+        <f t="shared" si="8"/>
+        <v>0.74898430000000005</v>
+      </c>
+      <c r="AQ16" s="3">
+        <f t="shared" si="9"/>
+        <v>0.24966170000000004</v>
+      </c>
+      <c r="AR16" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.24966129999999997</v>
+      </c>
+      <c r="AS16" s="3">
+        <f t="shared" si="11"/>
+        <v>0.24966129999999997</v>
+      </c>
+      <c r="AT16" s="3">
+        <f t="shared" si="12"/>
+        <v>-2.9999999998087112E-7</v>
+      </c>
+      <c r="AU16" s="3">
+        <f t="shared" si="13"/>
+        <v>0.4993223</v>
+      </c>
+      <c r="AV16" s="3">
+        <f t="shared" si="14"/>
+        <v>2.9999999998087112E-7</v>
+      </c>
+      <c r="AW16" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.4993223</v>
+      </c>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>6.7500000000000001E-9</v>
       </c>
@@ -1818,8 +2770,72 @@
       <c r="AF17" t="s">
         <v>1</v>
       </c>
+      <c r="AH17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999959999999999</v>
+      </c>
+      <c r="AI17" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49979639999999997</v>
+      </c>
+      <c r="AJ17" s="3">
+        <f t="shared" si="2"/>
+        <v>4.0000000001150227E-7</v>
+      </c>
+      <c r="AK17" s="3">
+        <f t="shared" si="3"/>
+        <v>0.50020359999999997</v>
+      </c>
+      <c r="AL17" s="4">
+        <f t="shared" si="4"/>
+        <v>0.24966145000000001</v>
+      </c>
+      <c r="AM17" s="4">
+        <f t="shared" si="5"/>
+        <v>0.74989854999999994</v>
+      </c>
+      <c r="AN17" s="4">
+        <f t="shared" si="6"/>
+        <v>0.25011855</v>
+      </c>
+      <c r="AO17" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.25011855</v>
+      </c>
+      <c r="AP17" s="4">
+        <f t="shared" si="8"/>
+        <v>0.74989854999999994</v>
+      </c>
+      <c r="AQ17" s="4">
+        <f t="shared" si="9"/>
+        <v>0.24966145000000001</v>
+      </c>
+      <c r="AR17" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.25011855</v>
+      </c>
+      <c r="AS17" s="4">
+        <f t="shared" si="11"/>
+        <v>0.25011855</v>
+      </c>
+      <c r="AT17" s="3">
+        <f t="shared" si="12"/>
+        <v>-2.9999999998087112E-7</v>
+      </c>
+      <c r="AU17" s="3">
+        <f t="shared" si="13"/>
+        <v>0.4993223</v>
+      </c>
+      <c r="AV17" s="3">
+        <f t="shared" si="14"/>
+        <v>2.9999999998087112E-7</v>
+      </c>
+      <c r="AW17" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.4993223</v>
+      </c>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>7.2500000000000004E-9</v>
       </c>
@@ -1913,8 +2929,72 @@
       <c r="AF18" t="s">
         <v>1</v>
       </c>
+      <c r="AH18" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999959999999999</v>
+      </c>
+      <c r="AI18" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49979639999999997</v>
+      </c>
+      <c r="AJ18" s="3">
+        <f t="shared" si="2"/>
+        <v>4.0000000001150227E-7</v>
+      </c>
+      <c r="AK18" s="3">
+        <f t="shared" si="3"/>
+        <v>0.50020359999999997</v>
+      </c>
+      <c r="AL18" s="3">
+        <f t="shared" si="4"/>
+        <v>0.24966145000000001</v>
+      </c>
+      <c r="AM18" s="3">
+        <f t="shared" si="5"/>
+        <v>0.74989854999999994</v>
+      </c>
+      <c r="AN18" s="3">
+        <f t="shared" si="6"/>
+        <v>0.25011855</v>
+      </c>
+      <c r="AO18" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.25011855</v>
+      </c>
+      <c r="AP18" s="3">
+        <f t="shared" si="8"/>
+        <v>0.74989854999999994</v>
+      </c>
+      <c r="AQ18" s="3">
+        <f t="shared" si="9"/>
+        <v>0.24966145000000001</v>
+      </c>
+      <c r="AR18" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.25011855</v>
+      </c>
+      <c r="AS18" s="3">
+        <f t="shared" si="11"/>
+        <v>0.25011855</v>
+      </c>
+      <c r="AT18" s="4">
+        <f t="shared" si="12"/>
+        <v>-1.5000000003206893E-7</v>
+      </c>
+      <c r="AU18" s="4">
+        <f t="shared" si="13"/>
+        <v>0.49993215000000002</v>
+      </c>
+      <c r="AV18" s="4">
+        <f t="shared" si="14"/>
+        <v>1.5000000003206893E-7</v>
+      </c>
+      <c r="AW18" s="4">
+        <f t="shared" si="15"/>
+        <v>-0.49993215000000002</v>
+      </c>
     </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>7.7499999999999999E-9</v>
       </c>
@@ -2008,8 +3088,72 @@
       <c r="AF19" t="s">
         <v>1</v>
       </c>
+      <c r="AH19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999959999999999</v>
+      </c>
+      <c r="AI19" s="3">
+        <f t="shared" si="1"/>
+        <v>0.49979639999999997</v>
+      </c>
+      <c r="AJ19" s="3">
+        <f t="shared" si="2"/>
+        <v>4.0000000001150227E-7</v>
+      </c>
+      <c r="AK19" s="3">
+        <f t="shared" si="3"/>
+        <v>0.50020359999999997</v>
+      </c>
+      <c r="AL19" s="4">
+        <f t="shared" si="4"/>
+        <v>0.24996584999999996</v>
+      </c>
+      <c r="AM19" s="4">
+        <f t="shared" si="5"/>
+        <v>0.74989815000000004</v>
+      </c>
+      <c r="AN19" s="4">
+        <f t="shared" si="6"/>
+        <v>0.24996615000000003</v>
+      </c>
+      <c r="AO19" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.24996615000000003</v>
+      </c>
+      <c r="AP19" s="4">
+        <f t="shared" si="8"/>
+        <v>0.74989815000000004</v>
+      </c>
+      <c r="AQ19" s="4">
+        <f t="shared" si="9"/>
+        <v>0.24996584999999996</v>
+      </c>
+      <c r="AR19" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.24996615000000003</v>
+      </c>
+      <c r="AS19" s="4">
+        <f t="shared" si="11"/>
+        <v>0.24996615000000003</v>
+      </c>
+      <c r="AT19" s="3">
+        <f t="shared" si="12"/>
+        <v>-1.5000000003206893E-7</v>
+      </c>
+      <c r="AU19" s="3">
+        <f t="shared" si="13"/>
+        <v>0.49993215000000002</v>
+      </c>
+      <c r="AV19" s="3">
+        <f t="shared" si="14"/>
+        <v>1.5000000003206893E-7</v>
+      </c>
+      <c r="AW19" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.49993215000000002</v>
+      </c>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>8.2499999999999994E-9</v>
       </c>
@@ -2103,8 +3247,72 @@
       <c r="AF20" t="s">
         <v>1</v>
       </c>
+      <c r="AH20" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AI20" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="AJ20" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK20" s="4">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="AL20" s="3">
+        <f t="shared" si="4"/>
+        <v>0.24996584999999996</v>
+      </c>
+      <c r="AM20" s="3">
+        <f t="shared" si="5"/>
+        <v>0.74989815000000004</v>
+      </c>
+      <c r="AN20" s="3">
+        <f t="shared" si="6"/>
+        <v>0.24996615000000003</v>
+      </c>
+      <c r="AO20" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.24996615000000003</v>
+      </c>
+      <c r="AP20" s="3">
+        <f t="shared" si="8"/>
+        <v>0.74989815000000004</v>
+      </c>
+      <c r="AQ20" s="3">
+        <f t="shared" si="9"/>
+        <v>0.24996584999999996</v>
+      </c>
+      <c r="AR20" s="3">
+        <f t="shared" si="10"/>
+        <v>-0.24996615000000003</v>
+      </c>
+      <c r="AS20" s="3">
+        <f t="shared" si="11"/>
+        <v>0.24996615000000003</v>
+      </c>
+      <c r="AT20" s="3">
+        <f t="shared" si="12"/>
+        <v>-1.5000000003206893E-7</v>
+      </c>
+      <c r="AU20" s="3">
+        <f t="shared" si="13"/>
+        <v>0.49993215000000002</v>
+      </c>
+      <c r="AV20" s="3">
+        <f t="shared" si="14"/>
+        <v>1.5000000003206893E-7</v>
+      </c>
+      <c r="AW20" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.49993215000000002</v>
+      </c>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:49" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>8.7500000000000006E-9</v>
       </c>
@@ -2197,6 +3405,70 @@
       </c>
       <c r="AF21" t="s">
         <v>1</v>
+      </c>
+      <c r="AH21" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AI21" s="3">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="AJ21" s="3">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK21" s="3">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="AL21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.24996605</v>
+      </c>
+      <c r="AM21" s="4">
+        <f t="shared" si="5"/>
+        <v>0.74999995000000008</v>
+      </c>
+      <c r="AN21" s="4">
+        <f t="shared" si="6"/>
+        <v>0.25001695000000002</v>
+      </c>
+      <c r="AO21" s="4">
+        <f t="shared" si="7"/>
+        <v>-0.25001695000000002</v>
+      </c>
+      <c r="AP21" s="4">
+        <f t="shared" si="8"/>
+        <v>0.74999995000000008</v>
+      </c>
+      <c r="AQ21" s="4">
+        <f t="shared" si="9"/>
+        <v>0.24996605</v>
+      </c>
+      <c r="AR21" s="4">
+        <f t="shared" si="10"/>
+        <v>-0.25001695000000002</v>
+      </c>
+      <c r="AS21" s="4">
+        <f t="shared" si="11"/>
+        <v>0.25001695000000002</v>
+      </c>
+      <c r="AT21" s="3">
+        <f t="shared" si="12"/>
+        <v>-1.5000000003206893E-7</v>
+      </c>
+      <c r="AU21" s="3">
+        <f t="shared" si="13"/>
+        <v>0.49993215000000002</v>
+      </c>
+      <c r="AV21" s="3">
+        <f t="shared" si="14"/>
+        <v>1.5000000003206893E-7</v>
+      </c>
+      <c r="AW21" s="3">
+        <f t="shared" si="15"/>
+        <v>-0.49993215000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Approximate transmission line models
</commit_message>
<xml_diff>
--- a/TestSignalIntegrity/FourPortTline.xlsx
+++ b/TestSignalIntegrity/FourPortTline.xlsx
@@ -174,7 +174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -182,6 +182,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -484,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AW21"/>
+  <dimension ref="B1:AW27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AL24" sqref="AL24"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,13 +620,13 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>6.6664130000000004</v>
       </c>
       <c r="F4" t="s">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="5">
         <v>-6.6664130000000004</v>
       </c>
       <c r="H4" t="s">
@@ -667,13 +668,13 @@
       <c r="T4" t="s">
         <v>0</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="5">
         <v>0.66667900000000002</v>
       </c>
       <c r="V4" t="s">
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="5">
         <v>0.33332099999999998</v>
       </c>
       <c r="X4" t="s">
@@ -790,25 +791,25 @@
       <c r="H5" t="s">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>-6.6667509999999996</v>
       </c>
       <c r="J5" t="s">
         <v>0</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="5">
         <v>6.6667509999999996</v>
       </c>
       <c r="L5" t="s">
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="5">
         <v>6.6667509999999996</v>
       </c>
       <c r="N5" t="s">
         <v>0</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="5">
         <v>-6.6667509999999996</v>
       </c>
       <c r="P5" t="s">
@@ -838,13 +839,13 @@
       <c r="X5" t="s">
         <v>1</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="5">
         <v>0.33334200000000003</v>
       </c>
       <c r="Z5" t="s">
         <v>1</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="5">
         <v>0</v>
       </c>
       <c r="AB5" t="s">
@@ -973,13 +974,13 @@
       <c r="P6" t="s">
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="5">
         <v>-4.4445290000000002</v>
       </c>
       <c r="R6" t="s">
         <v>0</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="5">
         <v>4.4445290000000002</v>
       </c>
       <c r="T6" t="s">
@@ -1009,13 +1010,13 @@
       <c r="AB6" t="s">
         <v>1</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="5">
         <v>0.22222600000000001</v>
       </c>
       <c r="AD6" t="s">
         <v>1</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="5">
         <v>-0.22222600000000001</v>
       </c>
       <c r="AF6" t="s">
@@ -1108,25 +1109,25 @@
       <c r="H7" t="s">
         <v>0</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="5">
         <v>-4.4445290000000002</v>
       </c>
       <c r="J7" t="s">
         <v>0</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="5">
         <v>4.4445290000000002</v>
       </c>
       <c r="L7" t="s">
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="5">
         <v>4.4445290000000002</v>
       </c>
       <c r="N7" t="s">
         <v>0</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="5">
         <v>-4.4445290000000002</v>
       </c>
       <c r="P7" t="s">
@@ -1156,13 +1157,13 @@
       <c r="X7" t="s">
         <v>1</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="5">
         <v>0.44445299999999999</v>
       </c>
       <c r="Z7" t="s">
         <v>1</v>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="5">
         <v>0</v>
       </c>
       <c r="AB7" t="s">
@@ -1255,13 +1256,13 @@
       <c r="D8" t="s">
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>5.1849309999999997</v>
       </c>
       <c r="F8" t="s">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
         <v>-5.1849309999999997</v>
       </c>
       <c r="H8" t="s">
@@ -1303,13 +1304,13 @@
       <c r="T8" t="s">
         <v>0</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="5">
         <v>0.74075299999999999</v>
       </c>
       <c r="V8" t="s">
         <v>1</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="5">
         <v>0.25924700000000001</v>
       </c>
       <c r="X8" t="s">
@@ -3469,6 +3470,12 @@
       <c r="AW21" s="3">
         <f t="shared" si="15"/>
         <v>-0.49993215000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:49" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <f>1/(4*AH1)*1000</f>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>